<commit_message>
1.新增 BudgetExecution 資料表 年份欄位 2.新增 BudgetExecution 前台程式 3.master page 調整
</commit_message>
<xml_diff>
--- a/ISTI_CityNavigation/Docs/DD.xlsx
+++ b/ISTI_CityNavigation/Docs/DD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WebProject\CityNavigation\ISTI_CityNavigation\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEAB9BB-36FE-4809-ACF5-2E92E55928C0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6B973E-D442-4F5C-8040-9BD75301CF5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="778" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="778" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="清單" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="852">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="855">
   <si>
     <t>成員基本資料</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2844,6 +2844,18 @@
   </si>
   <si>
     <t>Education</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>年</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B_Year</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nvarchar(5)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2930,7 +2942,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2982,13 +2994,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3302,7 +3317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -3313,10 +3328,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="19"/>
+      <c r="B1" s="18"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="str">
@@ -3538,22 +3553,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>365</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>364</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="13" t="s">
@@ -3892,22 +3907,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>403</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>402</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="13" t="s">
@@ -4218,22 +4233,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>457</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>456</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="13" t="s">
@@ -4648,22 +4663,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>509</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>508</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="13" t="s">
@@ -5110,22 +5125,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>536</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>535</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="13" t="s">
@@ -5382,22 +5397,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>565</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>564</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="13" t="s">
@@ -5666,22 +5681,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>605</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>604</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="13" t="s">
@@ -6034,22 +6049,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>659</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>658</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="13" t="s">
@@ -6486,22 +6501,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>687</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>686</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="13" t="s">
@@ -6769,22 +6784,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>740</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>739</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:8" ht="49.5">
       <c r="A3" s="13" t="s">
@@ -7214,22 +7229,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="2" t="s">
@@ -7453,22 +7468,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>840</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>839</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:8" ht="49.5">
       <c r="A3" s="12" t="s">
@@ -8195,22 +8210,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="2" t="s">
@@ -8310,10 +8325,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00A08E0-8C7E-4ECB-B481-93A833BA383B}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.375" defaultRowHeight="16.5"/>
@@ -8326,22 +8341,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="2" t="s">
@@ -8376,21 +8391,22 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>98</v>
+        <v>852</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
-      </c>
+        <v>853</v>
+      </c>
+      <c r="C5" s="17"/>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>854</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
         <v>4</v>
@@ -8398,10 +8414,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
@@ -8409,10 +8425,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
@@ -8420,10 +8436,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D9" t="s">
         <v>4</v>
@@ -8431,10 +8447,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" t="s">
         <v>4</v>
@@ -8442,10 +8458,10 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
@@ -8453,32 +8469,32 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D12" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
@@ -8486,23 +8502,34 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D15" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>33</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>97</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>13</v>
       </c>
     </row>
@@ -8534,22 +8561,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="2" t="s">
@@ -8819,22 +8846,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="2" t="s">
@@ -9016,22 +9043,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="2" t="s">
@@ -9213,22 +9240,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="2" t="s">
@@ -9983,22 +10010,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="20" t="s">
         <v>310</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>309</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="49.5">
       <c r="A3" s="2" t="s">

</xml_diff>